<commit_message>
update api import student course
</commit_message>
<xml_diff>
--- a/public/template/template_course.xlsx
+++ b/public/template/template_course.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiendam/Dev/Projects/student.resource.vnua/backend/public/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiendam/Dev/Projects/st.student-resource/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26251185-F55D-5C42-AF42-DC19A0811778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB973C9-504F-4E49-B541-FB4FDB7207EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>STT</t>
   </si>
@@ -48,51 +48,15 @@
     <t>Dân tộc</t>
   </si>
   <si>
-    <t>K67CNTTA</t>
-  </si>
-  <si>
-    <t>2022-2026</t>
-  </si>
-  <si>
     <t>Công nghệ thông tin</t>
   </si>
   <si>
-    <t>Đinh Hải Nam</t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>0357909299</t>
-  </si>
-  <si>
-    <t>Phùng Minh Ngọc Tuệ</t>
-  </si>
-  <si>
-    <t>0336114468</t>
-  </si>
-  <si>
-    <t>Đỗ Huy Việt Hùng</t>
-  </si>
-  <si>
     <t>Kinh</t>
   </si>
   <si>
-    <t>0785852666</t>
-  </si>
-  <si>
-    <t>Vũ Duy Hưng</t>
-  </si>
-  <si>
-    <t>0912153359</t>
-  </si>
-  <si>
-    <t>Trương Quang Nghĩa</t>
-  </si>
-  <si>
-    <t>0815348188</t>
-  </si>
-  <si>
     <t>Ngày sinh</t>
   </si>
   <si>
@@ -103,16 +67,137 @@
   </si>
   <si>
     <t>Niên khóa</t>
+  </si>
+  <si>
+    <t>Mã nhập học</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Địa chỉ báo tin</t>
+  </si>
+  <si>
+    <t>Họ tên bố</t>
+  </si>
+  <si>
+    <t>SĐT của bố</t>
+  </si>
+  <si>
+    <t>Họ tên mẹ</t>
+  </si>
+  <si>
+    <t>SĐT của mẹ</t>
+  </si>
+  <si>
+    <t>4PB4874</t>
+  </si>
+  <si>
+    <t>22/06/2006</t>
+  </si>
+  <si>
+    <t>K69CNTTA</t>
+  </si>
+  <si>
+    <t>2024-2028</t>
+  </si>
+  <si>
+    <t>4PB4876</t>
+  </si>
+  <si>
+    <t>13/03/2006</t>
+  </si>
+  <si>
+    <t>Thôn Thắng Trí,Minh Trí, Sóc Sơn, Hà nội</t>
+  </si>
+  <si>
+    <t>4PB4877</t>
+  </si>
+  <si>
+    <t>11/08/2006</t>
+  </si>
+  <si>
+    <t>Tày</t>
+  </si>
+  <si>
+    <t>Tổ 5, thị trấn Bằng Lũng, huyện Chợ Đồn, tỉnh Bắc Kan</t>
+  </si>
+  <si>
+    <t>Nguyễn Trường A</t>
+  </si>
+  <si>
+    <t>Dương Tuấn A</t>
+  </si>
+  <si>
+    <t>Hà Hoàng A</t>
+  </si>
+  <si>
+    <t>as@gmail.com</t>
+  </si>
+  <si>
+    <t>st@gmail.com</t>
+  </si>
+  <si>
+    <t>Dương Văn B</t>
+  </si>
+  <si>
+    <t>Hà Văn K</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị T</t>
+  </si>
+  <si>
+    <t>Hoàng Thị m</t>
+  </si>
+  <si>
+    <t>st.team@gmail.com</t>
+  </si>
+  <si>
+    <t>0979808408</t>
+  </si>
+  <si>
+    <t>0979808406</t>
+  </si>
+  <si>
+    <t>0979808407</t>
+  </si>
+  <si>
+    <t>0869919316</t>
+  </si>
+  <si>
+    <t>0869919314</t>
+  </si>
+  <si>
+    <t>0869919315</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,18 +238,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -440,18 +542,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
@@ -460,196 +562,228 @@
     <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2">
+        <v>698022</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2">
+        <v>375131069</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="C3" s="2">
+        <v>698032</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>869080314</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2">
+        <v>698043</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <v>671694</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3">
-        <v>38057</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2">
-        <v>672010</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="3">
-        <v>38087</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>671482</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3">
-        <v>37577</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>671503</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3">
-        <v>38215</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2">
-        <v>671719</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="3">
-        <v>38084</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="K4" s="2">
+        <v>878401446</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>